<commit_message>
overflow einlesen und beim vergleichen berücksichtigen
</commit_message>
<xml_diff>
--- a/src/test/resources/005 One-team-two-mhprojects-with-overflow.xlsx
+++ b/src/test/resources/005 One-team-two-mhprojects-with-overflow.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ProjektPortfolio\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="20625" windowHeight="8340"/>
   </bookViews>
@@ -78,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -113,13 +118,16 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -396,11 +404,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.875" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
@@ -745,10 +753,10 @@
         <v>42491</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C46">
-        <v>8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -756,10 +764,10 @@
         <v>42522</v>
       </c>
       <c r="B47">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C47">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -767,10 +775,10 @@
         <v>42552</v>
       </c>
       <c r="B48">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="C48">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -778,10 +786,10 @@
         <v>42583</v>
       </c>
       <c r="B49">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C49">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -789,10 +797,10 @@
         <v>42614</v>
       </c>
       <c r="B50">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -800,10 +808,10 @@
         <v>42644</v>
       </c>
       <c r="B51">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C51">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1003,7 +1011,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B71">
-        <v>1</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1039,7 +1047,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1051,7 +1059,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>